<commit_message>
data cleaning and quality assurance
</commit_message>
<xml_diff>
--- a/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
+++ b/Forage_Fish_Diet_Data_2013_2015_Final.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Desktop/nes-lter-fish-diet-isotope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E7E5F7-96E9-6240-B004-F0FDF02B71D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ACCD90-BD5C-C940-AFA5-067E09F920FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="17920" windowHeight="14700" activeTab="3" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="20260" windowHeight="14740" activeTab="1" xr2:uid="{20CBF2A6-5EEF-447F-A717-1AB3AC94F5B2}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTable" sheetId="1" r:id="rId1"/>
     <sheet name="ColumnHeaders" sheetId="2" r:id="rId2"/>
     <sheet name="ColumnHeaders_ordered" sheetId="6" r:id="rId3"/>
-    <sheet name="FishLookup" sheetId="5" r:id="rId4"/>
-    <sheet name="CategoricalVariables" sheetId="3" r:id="rId5"/>
-    <sheet name="Personnel" sheetId="4" r:id="rId6"/>
+    <sheet name="CategoricalVariables" sheetId="3" r:id="rId4"/>
+    <sheet name="Personnel" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DataTable!$A$1:$BF$503</definedName>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="364">
   <si>
     <t>Cruise</t>
   </si>
@@ -1283,21 +1282,6 @@
     <t>Expansion</t>
   </si>
   <si>
-    <t>Clupea harengus</t>
-  </si>
-  <si>
-    <t>Peprilus triacanthus</t>
-  </si>
-  <si>
-    <t>Scomber scombrus</t>
-  </si>
-  <si>
-    <t>Alosa aestivalis</t>
-  </si>
-  <si>
-    <t>Alosa pseudoharengus</t>
-  </si>
-  <si>
     <t>abbrevName_fish</t>
   </si>
   <si>
@@ -1338,21 +1322,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Alewife</t>
-  </si>
-  <si>
-    <t>Atlantic butterfish</t>
-  </si>
-  <si>
-    <t>Atlantic mackerel</t>
-  </si>
-  <si>
-    <t>Blueback herring</t>
-  </si>
-  <si>
-    <t>Atlantic herring</t>
   </si>
   <si>
     <t>Cruise that sample was collected during</t>
@@ -1431,6 +1400,27 @@
   </si>
   <si>
     <t>millimeter</t>
+  </si>
+  <si>
+    <t>Average depth of seafloor during sampling event</t>
+  </si>
+  <si>
+    <t>Length of the fish measured from the tip of the snout to the end of the middle caudal fin rays</t>
+  </si>
+  <si>
+    <t>Latitude at the start of the sample event</t>
+  </si>
+  <si>
+    <t>Longitude at the start of the sample event</t>
+  </si>
+  <si>
+    <t>Llopiz lab category of prey item</t>
+  </si>
+  <si>
+    <t>Unique number for fish specimen</t>
+  </si>
+  <si>
+    <t>average_depth</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1822,7 @@
   <dimension ref="A1:BE503"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -88900,8 +88890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19A1ABC-A786-414A-A468-0B39AD2E7808}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -88945,10 +88935,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D2" t="s">
         <v>250</v>
@@ -88959,10 +88949,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C3" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="D3" t="s">
         <v>252</v>
@@ -88976,10 +88966,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C4" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="D4" t="s">
         <v>250</v>
@@ -88990,10 +88980,10 @@
         <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C5" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="D5" t="s">
         <v>252</v>
@@ -89007,10 +88997,10 @@
         <v>242</v>
       </c>
       <c r="B6" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D6" t="s">
         <v>252</v>
@@ -89027,7 +89017,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D7" t="s">
         <v>252</v>
@@ -89041,10 +89031,10 @@
         <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C8" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="D8" t="s">
         <v>251</v>
@@ -89058,10 +89048,10 @@
         <v>204</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>363</v>
       </c>
       <c r="C9" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>252</v>
@@ -89075,13 +89065,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D10" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -89089,10 +89079,10 @@
         <v>206</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C11" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>252</v>
@@ -89106,10 +89096,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C12" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D12" t="s">
         <v>250</v>
@@ -89118,10 +89108,10 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C13" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>250</v>
@@ -89129,10 +89119,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C14" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>252</v>
@@ -89143,10 +89133,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C15" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>251</v>
@@ -89157,10 +89147,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>251</v>
@@ -89171,10 +89161,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C17" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>250</v>
@@ -89185,7 +89175,7 @@
         <v>297</v>
       </c>
       <c r="C18" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>250</v>
@@ -89193,10 +89183,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C19" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>250</v>
@@ -89207,7 +89197,7 @@
         <v>298</v>
       </c>
       <c r="C20" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>250</v>
@@ -89215,10 +89205,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C21" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>250</v>
@@ -89226,10 +89216,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C22" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>250</v>
@@ -89244,14 +89234,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269705B7-DB6F-CA4E-AC53-B891847B83EE}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -89280,10 +89271,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B2" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C2" t="s">
         <v>250</v>
@@ -89291,10 +89282,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C3" t="s">
         <v>252</v>
@@ -89305,10 +89296,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C4" t="s">
         <v>250</v>
@@ -89316,10 +89307,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="C5" t="s">
         <v>252</v>
@@ -89330,10 +89321,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="C6" t="s">
         <v>252</v>
@@ -89347,7 +89338,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C7" t="s">
         <v>252</v>
@@ -89358,10 +89349,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>363</v>
       </c>
       <c r="B8" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>252</v>
@@ -89372,35 +89363,35 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C9" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B10" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>252</v>
       </c>
       <c r="D10" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B11" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="C11" t="s">
         <v>250</v>
@@ -89408,10 +89399,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B12" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>250</v>
@@ -89419,10 +89410,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B13" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>252</v>
@@ -89433,10 +89424,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B14" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>250</v>
@@ -89444,10 +89435,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="C15" t="s">
         <v>251</v>
@@ -89458,10 +89449,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C16" t="s">
         <v>251</v>
@@ -89472,10 +89463,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B17" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C17" t="s">
         <v>251</v>
@@ -89486,10 +89477,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B18" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>250</v>
@@ -89497,10 +89488,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B19" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>250</v>
@@ -89511,7 +89502,7 @@
         <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>250</v>
@@ -89522,7 +89513,7 @@
         <v>298</v>
       </c>
       <c r="B21" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>250</v>
@@ -89530,10 +89521,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B22" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>250</v>
@@ -89548,110 +89539,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAB4A06-3B58-2942-A44D-EF1A30A01AC7}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>322</v>
-      </c>
-      <c r="B1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>317</v>
-      </c>
-      <c r="C2">
-        <v>161722</v>
-      </c>
-      <c r="D2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C3">
-        <v>172567</v>
-      </c>
-      <c r="D3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4">
-        <v>172414</v>
-      </c>
-      <c r="D4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>320</v>
-      </c>
-      <c r="C5">
-        <v>161703</v>
-      </c>
-      <c r="D5" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6">
-        <v>161706</v>
-      </c>
-      <c r="D6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1450A43-7CE0-8C4D-80E9-CDBE5E6D7720}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -89704,12 +89591,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043A2994-6F23-AA46-80A5-5A5F95B766AF}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>